<commit_message>
bulk add inventory and analytics
</commit_message>
<xml_diff>
--- a/frontend/public/templates/inventory-template.xlsx
+++ b/frontend/public/templates/inventory-template.xlsx
@@ -397,102 +397,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" customWidth="1" width="15"/>
+    <col min="1" max="1" customWidth="1" width="8"/>
     <col min="2" max="2" customWidth="1" width="15"/>
-    <col min="3" max="3" customWidth="1" width="15"/>
-    <col min="4" max="4" customWidth="1" width="15"/>
-    <col min="5" max="5" customWidth="1" width="15"/>
-    <col min="6" max="6" customWidth="1" width="15"/>
-    <col min="7" max="7" customWidth="1" width="15"/>
-    <col min="8" max="8" customWidth="1" width="15"/>
+    <col min="3" max="3" customWidth="1" width="12"/>
+    <col min="4" max="4" customWidth="1" width="12"/>
+    <col min="5" max="5" customWidth="1" width="12"/>
+    <col min="6" max="6" customWidth="1" width="12"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ARTIS CODE</v>
+        <v>SNO</v>
       </c>
       <c r="B1" t="str">
-        <v>DESIGN NAME</v>
+        <v>OUR CODE</v>
       </c>
       <c r="C1" t="str">
-        <v>SUPPLIER</v>
+        <v>OUT</v>
       </c>
       <c r="D1" t="str">
-        <v>OPENING STOCK</v>
+        <v>OUT</v>
       </c>
       <c r="E1" t="str">
-        <v>TRANSACTION TYPE</v>
+        <v>OUT</v>
       </c>
       <c r="F1" t="str">
-        <v>QUANTITY</v>
-      </c>
-      <c r="G1" t="str">
-        <v>DATE</v>
-      </c>
-      <c r="H1" t="str">
-        <v>NOTES</v>
+        <v>IN</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>901</v>
+        <v/>
       </c>
       <c r="B2" t="str">
-        <v>Sample Design</v>
+        <v/>
       </c>
       <c r="C2" t="str">
-        <v>MATCH GRAPHICS</v>
+        <v>30/10/2024</v>
       </c>
       <c r="D2" t="str">
-        <v>100</v>
+        <v>30/9/2024</v>
       </c>
       <c r="E2" t="str">
-        <v>IN</v>
+        <v>30/8/2024</v>
       </c>
       <c r="F2" t="str">
-        <v>50</v>
-      </c>
-      <c r="G2" t="str">
-        <v>2024-03-20</v>
-      </c>
-      <c r="H2" t="str">
-        <v>Initial stock</v>
+        <v>1/8/24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
         <v>901</v>
       </c>
-      <c r="B3" t="str">
-        <v>Sample Design</v>
-      </c>
       <c r="C3" t="str">
-        <v>MATCH GRAPHICS</v>
+        <v>21</v>
       </c>
       <c r="D3" t="str">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="E3" t="str">
-        <v>OUT</v>
+        <v>64</v>
       </c>
       <c r="F3" t="str">
-        <v>30</v>
-      </c>
-      <c r="G3" t="str">
-        <v>2024-03-21</v>
-      </c>
-      <c r="H3" t="str">
-        <v>Sales deduction</v>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>902</v>
+      </c>
+      <c r="C4" t="str">
+        <v>28</v>
+      </c>
+      <c r="D4" t="str">
+        <v>25</v>
+      </c>
+      <c r="E4" t="str">
+        <v>46</v>
+      </c>
+      <c r="F4" t="str">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <v>903</v>
+      </c>
+      <c r="C5" t="str">
+        <v>16</v>
+      </c>
+      <c r="D5" t="str">
+        <v>45</v>
+      </c>
+      <c r="E5" t="str">
+        <v>41</v>
+      </c>
+      <c r="F5" t="str">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>